<commit_message>
Forgor to save file in R Studio
</commit_message>
<xml_diff>
--- a/python/832-check/resultDemo.xlsx
+++ b/python/832-check/resultDemo.xlsx
@@ -458,29 +458,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Participant-Visit Bravo-1 was not found in the BioBank sheet.</t>
+          <t>Participant-Visit Charlie-4 was not found in the Visit Enrollment sheet.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BioBank</t>
+          <t>Visit Enrollment</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Participant-Visit Alpha-2 was not found in LV.</t>
+          <t>Participant-Visit Charlie-4 was not found in LV.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,12 +490,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Participant-Visit Bravo-2 was not found in the Visit Enrollment sheet.</t>
+          <t>Participant-Visit Alpha-2 was not found in LV.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Visit Enrollment</t>
+          <t>LabVantage</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-4 was not found in the Visit Enrollment sheet.</t>
+          <t>Participant-Visit Bravo-2 was not found in the Visit Enrollment sheet.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,34 +578,34 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-4 was not found in LV.</t>
+          <t>Participant-Visit Bravo-1 was not found in the BioBank sheet.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LabVantage</t>
+          <t>BioBank</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added when i made the ITN scripts
</commit_message>
<xml_diff>
--- a/python/832-check/resultDemo.xlsx
+++ b/python/832-check/resultDemo.xlsx
@@ -458,34 +458,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-4 was not found in the Visit Enrollment sheet.</t>
+          <t>Participant-Visit Alpha-2 was not found in LV.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Visit Enrollment</t>
+          <t>LabVantage</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-4 was not found in LV.</t>
+          <t>Participant-Visit Charlie-3 was not found in the BioBank sheet.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LabVantage</t>
+          <t>BioBank</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,19 +495,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-3 was not found in the BioBank sheet.</t>
+          <t>Participant-Visit Charlie-3 was not found in LV.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BioBank</t>
+          <t>LabVantage</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -524,78 +524,78 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Participant-Visit Charlie-3 was not found in LV.</t>
+          <t>Participant-Visit Bravo-1 was not found in the BioBank sheet.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LabVantage</t>
+          <t>BioBank</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Participant-Visit Alpha-2 was not found in LV.</t>
+          <t>Participant-Visit Charlie-4 was not found in the Visit Enrollment sheet.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LabVantage</t>
+          <t>Visit Enrollment</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Participant-Visit Bravo-2 was not found in the Visit Enrollment sheet.</t>
+          <t>Participant-Visit Charlie-4 was not found in LV.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Visit Enrollment</t>
+          <t>LabVantage</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Participant-Visit Bravo-1 was not found in the BioBank sheet.</t>
+          <t>Participant-Visit Bravo-2 was not found in the Visit Enrollment sheet.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BioBank</t>
+          <t>Visit Enrollment</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>

</xml_diff>